<commit_message>
Data model PR finalized: fixed PKs, os_lanc fact, os_selo bridge, import validation
</commit_message>
<xml_diff>
--- a/backend/temp/041619_tabela_de_lançamentos.xlsx
+++ b/backend/temp/041619_tabela_de_lançamentos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AnSata\Exportador Cajuru\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas Matos\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B3986A-B6AC-4594-9C6B-2D1C16330449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2957DFF-9D87-43CE-86EA-3002E2D36098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{53201F29-6539-4835-99E0-2983CC509DEA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{53201F29-6539-4835-99E0-2983CC509DEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabela de Lançamentos" sheetId="1" r:id="rId1"/>
@@ -1160,19 +1160,19 @@
     <t>Emprestimo</t>
   </si>
   <si>
-    <t>Lcto</t>
-  </si>
-  <si>
-    <t>Descrição</t>
-  </si>
-  <si>
-    <t>Inativo</t>
-  </si>
-  <si>
-    <t>Grupo  de Contas</t>
-  </si>
-  <si>
-    <t>Tipo_lanc</t>
+    <t>CodLcto</t>
+  </si>
+  <si>
+    <t>Descricao</t>
+  </si>
+  <si>
+    <t>status_inativo</t>
+  </si>
+  <si>
+    <t>grupodecontas</t>
+  </si>
+  <si>
+    <t>tipo_lanc</t>
   </si>
 </sst>
 </file>
@@ -1546,17 +1546,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1296EC34-56B5-4F40-A29C-E5FE8EF800C7}">
   <dimension ref="A1:E373"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="B115" sqref="B115"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>374</v>
       </c>
@@ -1573,7 +1575,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1584,7 +1586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1595,7 +1597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1609,7 +1611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1623,7 +1625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -1634,7 +1636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -1645,7 +1647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -1656,7 +1658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -1673,7 +1675,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -1687,7 +1689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -1701,7 +1703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -1712,7 +1714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
@@ -1723,7 +1725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -1740,7 +1742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
@@ -1757,7 +1759,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1774,7 +1776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
@@ -1791,7 +1793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
@@ -1808,7 +1810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
@@ -1825,7 +1827,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
@@ -1839,7 +1841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
@@ -1853,7 +1855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>22</v>
       </c>
@@ -1864,7 +1866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>23</v>
       </c>
@@ -1875,7 +1877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
@@ -1892,7 +1894,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>33</v>
       </c>
@@ -1903,7 +1905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>34</v>
       </c>
@@ -1914,7 +1916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>35</v>
       </c>
@@ -1925,7 +1927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>36</v>
       </c>
@@ -1936,7 +1938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>51</v>
       </c>
@@ -1944,7 +1946,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>52</v>
       </c>
@@ -1952,7 +1954,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>53</v>
       </c>
@@ -1960,7 +1962,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>54</v>
       </c>
@@ -1968,7 +1970,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>55</v>
       </c>
@@ -1976,7 +1978,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>101</v>
       </c>
@@ -1993,7 +1995,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>102</v>
       </c>
@@ -2010,7 +2012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>103</v>
       </c>
@@ -2027,7 +2029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>104</v>
       </c>
@@ -2044,7 +2046,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>105</v>
       </c>
@@ -2061,7 +2063,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>106</v>
       </c>
@@ -2078,7 +2080,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>107</v>
       </c>
@@ -2095,7 +2097,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>108</v>
       </c>
@@ -2112,7 +2114,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>109</v>
       </c>
@@ -2129,7 +2131,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>111</v>
       </c>
@@ -2146,7 +2148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>113</v>
       </c>
@@ -2163,7 +2165,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>114</v>
       </c>
@@ -2180,7 +2182,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>115</v>
       </c>
@@ -2197,7 +2199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>116</v>
       </c>
@@ -2214,7 +2216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>117</v>
       </c>
@@ -2231,7 +2233,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>120</v>
       </c>
@@ -2248,7 +2250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>121</v>
       </c>
@@ -2265,7 +2267,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>122</v>
       </c>
@@ -2282,7 +2284,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>123</v>
       </c>
@@ -2299,7 +2301,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>126</v>
       </c>
@@ -2316,7 +2318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>133</v>
       </c>
@@ -2333,7 +2335,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>134</v>
       </c>
@@ -2350,7 +2352,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>135</v>
       </c>
@@ -2367,7 +2369,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>136</v>
       </c>
@@ -2384,7 +2386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>137</v>
       </c>
@@ -2401,7 +2403,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>138</v>
       </c>
@@ -2418,7 +2420,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>140</v>
       </c>
@@ -2435,7 +2437,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>143</v>
       </c>
@@ -2452,7 +2454,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>144</v>
       </c>
@@ -2469,7 +2471,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>145</v>
       </c>
@@ -2486,7 +2488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>149</v>
       </c>
@@ -2503,7 +2505,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>150</v>
       </c>
@@ -2520,7 +2522,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>151</v>
       </c>
@@ -2537,7 +2539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>161</v>
       </c>
@@ -2554,7 +2556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>163</v>
       </c>
@@ -2568,7 +2570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>165</v>
       </c>
@@ -2585,7 +2587,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>168</v>
       </c>
@@ -2599,7 +2601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>173</v>
       </c>
@@ -2616,7 +2618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>176</v>
       </c>
@@ -2633,7 +2635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>183</v>
       </c>
@@ -2647,7 +2649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>184</v>
       </c>
@@ -2664,7 +2666,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>186</v>
       </c>
@@ -2681,7 +2683,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>189</v>
       </c>
@@ -2698,7 +2700,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>190</v>
       </c>
@@ -2712,7 +2714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>191</v>
       </c>
@@ -2729,7 +2731,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>216</v>
       </c>
@@ -2746,7 +2748,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>218</v>
       </c>
@@ -2763,7 +2765,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>222</v>
       </c>
@@ -2780,7 +2782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>239</v>
       </c>
@@ -2797,7 +2799,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>262</v>
       </c>
@@ -2811,7 +2813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>263</v>
       </c>
@@ -2825,7 +2827,7 @@
         <v>211602</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>267</v>
       </c>
@@ -2842,7 +2844,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>268</v>
       </c>
@@ -2859,7 +2861,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>269</v>
       </c>
@@ -2876,7 +2878,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>297</v>
       </c>
@@ -2893,7 +2895,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>303</v>
       </c>
@@ -2910,7 +2912,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>304</v>
       </c>
@@ -2924,7 +2926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>323</v>
       </c>
@@ -2941,7 +2943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>326</v>
       </c>
@@ -2958,7 +2960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>332</v>
       </c>
@@ -2972,7 +2974,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>366</v>
       </c>
@@ -2989,7 +2991,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>370</v>
       </c>
@@ -3003,7 +3005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>371</v>
       </c>
@@ -3020,7 +3022,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>372</v>
       </c>
@@ -3037,7 +3039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>373</v>
       </c>
@@ -3051,7 +3053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>375</v>
       </c>
@@ -3068,7 +3070,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>376</v>
       </c>
@@ -3082,7 +3084,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>401</v>
       </c>
@@ -3096,7 +3098,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>438</v>
       </c>
@@ -3110,7 +3112,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>461</v>
       </c>
@@ -3127,7 +3129,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>482</v>
       </c>
@@ -3141,7 +3143,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>485</v>
       </c>
@@ -3155,7 +3157,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>486</v>
       </c>
@@ -3169,7 +3171,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>488</v>
       </c>
@@ -3183,7 +3185,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>489</v>
       </c>
@@ -3197,7 +3199,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>490</v>
       </c>
@@ -3211,7 +3213,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>491</v>
       </c>
@@ -3228,7 +3230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>499</v>
       </c>
@@ -3245,7 +3247,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>505</v>
       </c>
@@ -3259,7 +3261,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>520</v>
       </c>
@@ -3273,7 +3275,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>521</v>
       </c>
@@ -3290,7 +3292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>522</v>
       </c>
@@ -3307,7 +3309,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>523</v>
       </c>
@@ -3324,7 +3326,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>528</v>
       </c>
@@ -3341,7 +3343,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>529</v>
       </c>
@@ -3358,7 +3360,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>530</v>
       </c>
@@ -3375,7 +3377,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>536</v>
       </c>
@@ -3392,7 +3394,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>537</v>
       </c>
@@ -3409,7 +3411,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>538</v>
       </c>
@@ -3426,7 +3428,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>539</v>
       </c>
@@ -3443,7 +3445,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>540</v>
       </c>
@@ -3460,7 +3462,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>541</v>
       </c>
@@ -3477,7 +3479,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>562</v>
       </c>
@@ -3494,7 +3496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>563</v>
       </c>
@@ -3511,7 +3513,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>564</v>
       </c>
@@ -3528,7 +3530,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>565</v>
       </c>
@@ -3545,7 +3547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>566</v>
       </c>
@@ -3562,7 +3564,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>567</v>
       </c>
@@ -3579,7 +3581,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>568</v>
       </c>
@@ -3593,7 +3595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>569</v>
       </c>
@@ -3610,7 +3612,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>572</v>
       </c>
@@ -3627,7 +3629,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>573</v>
       </c>
@@ -3644,7 +3646,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>574</v>
       </c>
@@ -3661,7 +3663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>575</v>
       </c>
@@ -3678,7 +3680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>576</v>
       </c>
@@ -3692,7 +3694,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>577</v>
       </c>
@@ -3709,7 +3711,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>578</v>
       </c>
@@ -3726,7 +3728,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>579</v>
       </c>
@@ -3743,7 +3745,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>580</v>
       </c>
@@ -3760,7 +3762,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>581</v>
       </c>
@@ -3774,7 +3776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>582</v>
       </c>
@@ -3791,7 +3793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>583</v>
       </c>
@@ -3808,7 +3810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>584</v>
       </c>
@@ -3825,7 +3827,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>585</v>
       </c>
@@ -3839,7 +3841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>586</v>
       </c>
@@ -3853,7 +3855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>587</v>
       </c>
@@ -3867,7 +3869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>588</v>
       </c>
@@ -3881,7 +3883,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>589</v>
       </c>
@@ -3895,7 +3897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>590</v>
       </c>
@@ -3912,7 +3914,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>591</v>
       </c>
@@ -3929,7 +3931,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>592</v>
       </c>
@@ -3946,7 +3948,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>593</v>
       </c>
@@ -3963,7 +3965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>594</v>
       </c>
@@ -3977,7 +3979,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>595</v>
       </c>
@@ -3991,7 +3993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>596</v>
       </c>
@@ -4005,7 +4007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>597</v>
       </c>
@@ -4019,7 +4021,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>598</v>
       </c>
@@ -4033,7 +4035,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>599</v>
       </c>
@@ -4050,7 +4052,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>600</v>
       </c>
@@ -4064,7 +4066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>601</v>
       </c>
@@ -4081,7 +4083,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>602</v>
       </c>
@@ -4095,7 +4097,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>603</v>
       </c>
@@ -4112,7 +4114,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>604</v>
       </c>
@@ -4126,7 +4128,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>605</v>
       </c>
@@ -4140,7 +4142,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>606</v>
       </c>
@@ -4154,7 +4156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>607</v>
       </c>
@@ -4171,7 +4173,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>608</v>
       </c>
@@ -4188,7 +4190,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>609</v>
       </c>
@@ -4205,7 +4207,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>610</v>
       </c>
@@ -4222,7 +4224,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>611</v>
       </c>
@@ -4239,7 +4241,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>612</v>
       </c>
@@ -4256,7 +4258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>613</v>
       </c>
@@ -4270,7 +4272,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>614</v>
       </c>
@@ -4284,7 +4286,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>615</v>
       </c>
@@ -4298,7 +4300,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>616</v>
       </c>
@@ -4312,7 +4314,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>617</v>
       </c>
@@ -4329,7 +4331,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>618</v>
       </c>
@@ -4346,7 +4348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>619</v>
       </c>
@@ -4360,7 +4362,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>620</v>
       </c>
@@ -4377,7 +4379,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>622</v>
       </c>
@@ -4394,7 +4396,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>623</v>
       </c>
@@ -4411,7 +4413,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>625</v>
       </c>
@@ -4428,7 +4430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>626</v>
       </c>
@@ -4445,7 +4447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>627</v>
       </c>
@@ -4459,7 +4461,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>628</v>
       </c>
@@ -4473,7 +4475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>629</v>
       </c>
@@ -4487,7 +4489,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>630</v>
       </c>
@@ -4504,7 +4506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>631</v>
       </c>
@@ -4521,7 +4523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>632</v>
       </c>
@@ -4538,7 +4540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>633</v>
       </c>
@@ -4552,7 +4554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>634</v>
       </c>
@@ -4569,7 +4571,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>635</v>
       </c>
@@ -4586,7 +4588,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>636</v>
       </c>
@@ -4603,7 +4605,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>637</v>
       </c>
@@ -4617,7 +4619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>638</v>
       </c>
@@ -4634,7 +4636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>639</v>
       </c>
@@ -4651,7 +4653,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>640</v>
       </c>
@@ -4668,7 +4670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>641</v>
       </c>
@@ -4685,7 +4687,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>642</v>
       </c>
@@ -4699,7 +4701,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>643</v>
       </c>
@@ -4716,7 +4718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>644</v>
       </c>
@@ -4733,7 +4735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>645</v>
       </c>
@@ -4747,7 +4749,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>646</v>
       </c>
@@ -4764,7 +4766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>647</v>
       </c>
@@ -4781,7 +4783,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>648</v>
       </c>
@@ -4798,7 +4800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>649</v>
       </c>
@@ -4815,7 +4817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>650</v>
       </c>
@@ -4832,7 +4834,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>651</v>
       </c>
@@ -4849,7 +4851,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>652</v>
       </c>
@@ -4866,7 +4868,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>653</v>
       </c>
@@ -4880,7 +4882,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>654</v>
       </c>
@@ -4894,7 +4896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>655</v>
       </c>
@@ -4911,7 +4913,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>656</v>
       </c>
@@ -4928,7 +4930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>657</v>
       </c>
@@ -4945,7 +4947,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>658</v>
       </c>
@@ -4962,7 +4964,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>659</v>
       </c>
@@ -4979,7 +4981,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>660</v>
       </c>
@@ -4993,7 +4995,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>661</v>
       </c>
@@ -5007,7 +5009,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>662</v>
       </c>
@@ -5024,7 +5026,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>663</v>
       </c>
@@ -5038,7 +5040,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>664</v>
       </c>
@@ -5052,7 +5054,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>665</v>
       </c>
@@ -5066,7 +5068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>666</v>
       </c>
@@ -5080,7 +5082,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>667</v>
       </c>
@@ -5094,7 +5096,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>668</v>
       </c>
@@ -5111,7 +5113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>669</v>
       </c>
@@ -5128,7 +5130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>670</v>
       </c>
@@ -5145,7 +5147,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>671</v>
       </c>
@@ -5162,7 +5164,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>672</v>
       </c>
@@ -5176,7 +5178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>673</v>
       </c>
@@ -5193,7 +5195,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>674</v>
       </c>
@@ -5210,7 +5212,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>675</v>
       </c>
@@ -5224,7 +5226,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>676</v>
       </c>
@@ -5241,7 +5243,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>677</v>
       </c>
@@ -5255,7 +5257,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>678</v>
       </c>
@@ -5272,7 +5274,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>679</v>
       </c>
@@ -5286,7 +5288,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>680</v>
       </c>
@@ -5303,7 +5305,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>681</v>
       </c>
@@ -5317,7 +5319,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>682</v>
       </c>
@@ -5334,7 +5336,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>683</v>
       </c>
@@ -5348,7 +5350,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>684</v>
       </c>
@@ -5365,7 +5367,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>685</v>
       </c>
@@ -5382,7 +5384,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>686</v>
       </c>
@@ -5396,7 +5398,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>687</v>
       </c>
@@ -5413,7 +5415,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>688</v>
       </c>
@@ -5427,7 +5429,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>689</v>
       </c>
@@ -5441,7 +5443,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>690</v>
       </c>
@@ -5455,7 +5457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>691</v>
       </c>
@@ -5469,7 +5471,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>692</v>
       </c>
@@ -5486,7 +5488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>693</v>
       </c>
@@ -5503,7 +5505,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>694</v>
       </c>
@@ -5517,7 +5519,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>695</v>
       </c>
@@ -5531,7 +5533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>696</v>
       </c>
@@ -5545,7 +5547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>697</v>
       </c>
@@ -5559,7 +5561,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>698</v>
       </c>
@@ -5576,7 +5578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>699</v>
       </c>
@@ -5590,7 +5592,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>700</v>
       </c>
@@ -5607,7 +5609,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>701</v>
       </c>
@@ -5624,7 +5626,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>702</v>
       </c>
@@ -5638,7 +5640,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>703</v>
       </c>
@@ -5655,7 +5657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>704</v>
       </c>
@@ -5672,7 +5674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>705</v>
       </c>
@@ -5689,7 +5691,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>706</v>
       </c>
@@ -5706,7 +5708,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>707</v>
       </c>
@@ -5720,7 +5722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>708</v>
       </c>
@@ -5737,7 +5739,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>709</v>
       </c>
@@ -5754,7 +5756,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>710</v>
       </c>
@@ -5771,7 +5773,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>711</v>
       </c>
@@ -5788,7 +5790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>712</v>
       </c>
@@ -5805,7 +5807,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>713</v>
       </c>
@@ -5822,7 +5824,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>714</v>
       </c>
@@ -5839,7 +5841,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>715</v>
       </c>
@@ -5856,7 +5858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>716</v>
       </c>
@@ -5873,7 +5875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>717</v>
       </c>
@@ -5890,7 +5892,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>718</v>
       </c>
@@ -5907,7 +5909,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>719</v>
       </c>
@@ -5924,7 +5926,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>720</v>
       </c>
@@ -5941,7 +5943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>721</v>
       </c>
@@ -5958,7 +5960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>722</v>
       </c>
@@ -5975,7 +5977,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>723</v>
       </c>
@@ -5992,7 +5994,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>724</v>
       </c>
@@ -6009,7 +6011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>725</v>
       </c>
@@ -6026,7 +6028,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>726</v>
       </c>
@@ -6043,7 +6045,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>727</v>
       </c>
@@ -6060,7 +6062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>728</v>
       </c>
@@ -6077,7 +6079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>729</v>
       </c>
@@ -6094,7 +6096,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>730</v>
       </c>
@@ -6111,7 +6113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>731</v>
       </c>
@@ -6128,7 +6130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>732</v>
       </c>
@@ -6145,7 +6147,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>733</v>
       </c>
@@ -6162,7 +6164,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>734</v>
       </c>
@@ -6179,7 +6181,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>735</v>
       </c>
@@ -6196,7 +6198,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>736</v>
       </c>
@@ -6213,7 +6215,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>737</v>
       </c>
@@ -6230,7 +6232,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>738</v>
       </c>
@@ -6247,7 +6249,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>739</v>
       </c>
@@ -6264,7 +6266,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>740</v>
       </c>
@@ -6281,7 +6283,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>741</v>
       </c>
@@ -6298,7 +6300,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>742</v>
       </c>
@@ -6315,7 +6317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>743</v>
       </c>
@@ -6332,7 +6334,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>744</v>
       </c>
@@ -6349,7 +6351,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>745</v>
       </c>
@@ -6366,7 +6368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>746</v>
       </c>
@@ -6383,7 +6385,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>747</v>
       </c>
@@ -6400,7 +6402,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>748</v>
       </c>
@@ -6417,7 +6419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>749</v>
       </c>
@@ -6434,7 +6436,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>750</v>
       </c>
@@ -6451,7 +6453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>751</v>
       </c>
@@ -6468,7 +6470,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>752</v>
       </c>
@@ -6485,7 +6487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>753</v>
       </c>
@@ -6502,7 +6504,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>754</v>
       </c>
@@ -6519,7 +6521,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>755</v>
       </c>
@@ -6536,7 +6538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>756</v>
       </c>
@@ -6553,7 +6555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>757</v>
       </c>
@@ -6570,7 +6572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>758</v>
       </c>
@@ -6587,7 +6589,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>759</v>
       </c>
@@ -6604,7 +6606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>760</v>
       </c>
@@ -6621,7 +6623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>761</v>
       </c>
@@ -6638,7 +6640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>762</v>
       </c>
@@ -6655,7 +6657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>763</v>
       </c>
@@ -6672,7 +6674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>764</v>
       </c>
@@ -6689,7 +6691,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>765</v>
       </c>
@@ -6706,7 +6708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>766</v>
       </c>
@@ -6723,7 +6725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>767</v>
       </c>
@@ -6740,7 +6742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>768</v>
       </c>
@@ -6757,7 +6759,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>769</v>
       </c>
@@ -6774,7 +6776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>770</v>
       </c>
@@ -6791,7 +6793,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>771</v>
       </c>
@@ -6808,7 +6810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>772</v>
       </c>
@@ -6825,7 +6827,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>773</v>
       </c>
@@ -6842,7 +6844,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>774</v>
       </c>
@@ -6859,7 +6861,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>775</v>
       </c>
@@ -6876,7 +6878,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>776</v>
       </c>
@@ -6893,7 +6895,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>777</v>
       </c>
@@ -6910,7 +6912,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>778</v>
       </c>
@@ -6927,7 +6929,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>779</v>
       </c>
@@ -6944,7 +6946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>780</v>
       </c>
@@ -6961,7 +6963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>781</v>
       </c>
@@ -6978,7 +6980,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>782</v>
       </c>
@@ -6995,7 +6997,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>783</v>
       </c>
@@ -7012,7 +7014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>784</v>
       </c>
@@ -7029,7 +7031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>785</v>
       </c>
@@ -7046,7 +7048,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>786</v>
       </c>
@@ -7063,7 +7065,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>787</v>
       </c>
@@ -7080,7 +7082,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>788</v>
       </c>
@@ -7097,7 +7099,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>789</v>
       </c>
@@ -7114,7 +7116,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>790</v>
       </c>
@@ -7131,7 +7133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>791</v>
       </c>
@@ -7148,7 +7150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>792</v>
       </c>
@@ -7165,7 +7167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>793</v>
       </c>
@@ -7182,7 +7184,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>794</v>
       </c>
@@ -7199,7 +7201,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>795</v>
       </c>
@@ -7216,7 +7218,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>796</v>
       </c>
@@ -7233,7 +7235,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>797</v>
       </c>
@@ -7247,7 +7249,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>798</v>
       </c>
@@ -7264,7 +7266,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>799</v>
       </c>
@@ -7281,7 +7283,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>800</v>
       </c>
@@ -7298,7 +7300,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>801</v>
       </c>
@@ -7315,7 +7317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>802</v>
       </c>
@@ -7332,7 +7334,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>803</v>
       </c>
@@ -7349,7 +7351,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>804</v>
       </c>
@@ -7366,7 +7368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>805</v>
       </c>
@@ -7380,7 +7382,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>806</v>
       </c>
@@ -7397,7 +7399,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>807</v>
       </c>
@@ -7414,7 +7416,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>808</v>
       </c>
@@ -7431,7 +7433,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>809</v>
       </c>
@@ -7448,7 +7450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>810</v>
       </c>
@@ -7465,7 +7467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>811</v>
       </c>
@@ -7482,7 +7484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>812</v>
       </c>
@@ -7499,7 +7501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>813</v>
       </c>

</xml_diff>